<commit_message>
some changes, i don't know what are they
</commit_message>
<xml_diff>
--- a/СЛАУ Метод Гаусса.xlsx
+++ b/СЛАУ Метод Гаусса.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Boris\Documents\MIREA\Course2\Vychmat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{485C69C5-350B-4E35-ACB2-7CE106C7B8BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E80E17C-1415-46D6-8470-D4917B8CF87E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="720" windowWidth="23490" windowHeight="15480" xr2:uid="{B70C56F0-9291-4471-95F3-619E217BE479}"/>
+    <workbookView xWindow="30" yWindow="0" windowWidth="23490" windowHeight="15480" xr2:uid="{B70C56F0-9291-4471-95F3-619E217BE479}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -737,7 +737,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1114,7 +1114,7 @@
         <v>-0.49999999999999711</v>
       </c>
       <c r="O18" s="25" t="str">
-        <f>IF(INT(M18)=M18,M18,TEXT(M18,"###/###"))</f>
+        <f>IF(INT(M18)=M18,TEXT(M18,"#"),TEXT(M18,"###/###"))</f>
         <v>-1/2</v>
       </c>
     </row>
@@ -1159,7 +1159,7 @@
         <v>4.9999999999999911</v>
       </c>
       <c r="O19" s="25" t="str">
-        <f t="shared" ref="O19:O20" si="24">IF(INT(M19)=M19,M19,TEXT(M19,"###/###"))</f>
+        <f t="shared" ref="O19:O20" si="24">IF(INT(M19)=M19,TEXT(M19,"#"),TEXT(M19,"###/###"))</f>
         <v>5/1</v>
       </c>
     </row>

</xml_diff>